<commit_message>
Added examples to the documentation of Get-functions for technical reports.
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/ex1/tables/mv_item.xlsx
+++ b/tests/testthat/fixtures/ex1/tables/mv_item.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -37,6 +37,18 @@
   </si>
   <si>
     <t xml:space="preserve">NR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AZ</t>
   </si>
   <si>
     <t xml:space="preserve">ALL</t>
@@ -504,13 +516,25 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -531,15 +555,27 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
         <v>3.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
@@ -560,15 +596,27 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
         <v>4.3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
@@ -589,15 +637,27 @@
         <v>0.5</v>
       </c>
       <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
         <v>3.5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
@@ -618,15 +678,27 @@
         <v>0.9</v>
       </c>
       <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
         <v>4.6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
@@ -647,15 +719,27 @@
         <v>1.6</v>
       </c>
       <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
         <v>5.1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
@@ -676,15 +760,27 @@
         <v>2.2</v>
       </c>
       <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
@@ -705,15 +801,27 @@
         <v>3.6</v>
       </c>
       <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
         <v>7.2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
@@ -734,15 +842,27 @@
         <v>4.6</v>
       </c>
       <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
         <v>8.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C10" t="n">
         <v>9</v>
@@ -763,15 +883,27 @@
         <v>6.2</v>
       </c>
       <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
         <v>9.1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
@@ -792,15 +924,27 @@
         <v>10.2</v>
       </c>
       <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
         <v>13.6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C12" t="n">
         <v>11</v>
@@ -821,15 +965,27 @@
         <v>14.7</v>
       </c>
       <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
         <v>18.4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C13" t="n">
         <v>12</v>
@@ -850,15 +1006,27 @@
         <v>22.2</v>
       </c>
       <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C14" t="n">
         <v>13</v>
@@ -879,15 +1047,27 @@
         <v>30.4</v>
       </c>
       <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
         <v>34.5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
@@ -908,15 +1088,27 @@
         <v>44.4</v>
       </c>
       <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
         <v>46.8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C16" t="n">
         <v>15</v>
@@ -937,6 +1129,18 @@
         <v>65.9</v>
       </c>
       <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
         <v>66.6</v>
       </c>
     </row>
@@ -959,19 +1163,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2">
@@ -1079,18 +1283,98 @@
         <v>8</v>
       </c>
       <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="n">
         <v>17.11</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C11" t="n">
         <v>18.72</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D11" t="n">
         <v>8.5</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E11" t="n">
         <v>3.5</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F11" t="n">
         <v>66.6</v>
       </c>
     </row>

</xml_diff>